<commit_message>
Update project with derived variables, docgen improvements, and date handling
</commit_message>
<xml_diff>
--- a/intake.xlsx
+++ b/intake.xlsx
@@ -507,6 +507,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <tabColor indexed="2"/>
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
@@ -567,7 +568,7 @@
       <c r="A3" s="9" t="n"/>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>defendantcaption</t>
+          <t>CCID</t>
         </is>
       </c>
       <c r="C3" s="10" t="inlineStr"/>
@@ -578,7 +579,7 @@
       </c>
       <c r="E3" s="9" t="inlineStr">
         <is>
-          <t>combined names of all defendants, E.g. "John Smith and Jane Smith"</t>
+          <t>Client's creditor number.</t>
         </is>
       </c>
     </row>
@@ -586,7 +587,7 @@
       <c r="A4" s="9" t="n"/>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>jurisdiction</t>
+          <t>XX25</t>
         </is>
       </c>
       <c r="C4" s="10" t="inlineStr"/>
@@ -597,7 +598,7 @@
       </c>
       <c r="E4" s="9" t="inlineStr">
         <is>
-          <t>County/District</t>
+          <t>caption number, don't include CI/JV etc. just "25-101"</t>
         </is>
       </c>
     </row>
@@ -605,7 +606,7 @@
       <c r="A5" s="9" t="n"/>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>venue</t>
+          <t>affirmdefplrl</t>
         </is>
       </c>
       <c r="C5" s="10" t="inlineStr"/>
@@ -616,37 +617,45 @@
       </c>
       <c r="E5" s="9" t="inlineStr">
         <is>
-          <t>the county name, e.g. "Garfield"</t>
+          <t>Whether more than one Aff Def, type s or leave blank.</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="9" t="inlineStr">
-        <is>
-          <t>Client</t>
-        </is>
-      </c>
-      <c r="B6" s="9" t="n"/>
-      <c r="C6" s="11" t="n"/>
-      <c r="D6" s="9" t="n"/>
-      <c r="E6" s="9" t="n"/>
+      <c r="A6" s="9" t="n"/>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>ccid</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr"/>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
+        <is>
+          <t>Client's specific matter/creditor number.</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="9" t="n"/>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>birthdate</t>
+          <t>clients</t>
         </is>
       </c>
       <c r="C7" s="11" t="inlineStr"/>
       <c r="D7" s="9" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="E7" s="9" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>In letters, pleadings, etc. you would say my clients or my client; type s for multiple clients.</t>
         </is>
       </c>
     </row>
@@ -654,7 +663,7 @@
       <c r="A8" s="9" t="n"/>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>firstname</t>
+          <t>defendantplural</t>
         </is>
       </c>
       <c r="C8" s="10" t="inlineStr"/>
@@ -665,7 +674,7 @@
       </c>
       <c r="E8" s="9" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>Pluralizes defendant vs defendants; type s or leave empty.</t>
         </is>
       </c>
     </row>
@@ -673,7 +682,7 @@
       <c r="A9" s="9" t="n"/>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>lastname</t>
+          <t>jurisdiction</t>
         </is>
       </c>
       <c r="C9" s="10" t="inlineStr"/>
@@ -684,7 +693,7 @@
       </c>
       <c r="E9" s="9" t="inlineStr">
         <is>
-          <t>v</t>
+          <t>County/District</t>
         </is>
       </c>
     </row>
@@ -692,7 +701,7 @@
       <c r="A10" s="9" t="n"/>
       <c r="B10" s="9" t="inlineStr">
         <is>
-          <t>spousefirstname</t>
+          <t>plaintiffattorneyemail</t>
         </is>
       </c>
       <c r="C10" s="10" t="inlineStr"/>
@@ -703,7 +712,7 @@
       </c>
       <c r="E10" s="9" t="inlineStr">
         <is>
-          <t>Lauren</t>
+          <t>Plaintiff's OC's email</t>
         </is>
       </c>
     </row>
@@ -711,7 +720,7 @@
       <c r="A11" s="9" t="n"/>
       <c r="B11" s="9" t="inlineStr">
         <is>
-          <t>spouselastname</t>
+          <t>plaintiffattorneyofrecord</t>
         </is>
       </c>
       <c r="C11" s="10" t="inlineStr"/>
@@ -722,7 +731,7 @@
       </c>
       <c r="E11" s="9" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>Email for OC</t>
         </is>
       </c>
     </row>
@@ -730,7 +739,7 @@
       <c r="A12" s="9" t="n"/>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>spousenfirstnameame</t>
+          <t>plaintiffbusPhone</t>
         </is>
       </c>
       <c r="C12" s="10" t="inlineStr"/>
@@ -741,26 +750,34 @@
       </c>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>x</t>
+          <t>Plaintiff's OC's firm's business number to speak to OC.</t>
         </is>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1" s="4">
-      <c r="A13" s="9" t="inlineStr">
-        <is>
-          <t>Internal</t>
-        </is>
-      </c>
-      <c r="B13" s="9" t="n"/>
-      <c r="C13" s="10" t="n"/>
-      <c r="D13" s="9" t="n"/>
-      <c r="E13" s="9" t="n"/>
+      <c r="A13" s="9" t="n"/>
+      <c r="B13" s="9" t="inlineStr">
+        <is>
+          <t>plaintiffbusphone</t>
+        </is>
+      </c>
+      <c r="C13" s="10" t="inlineStr"/>
+      <c r="D13" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E13" s="9" t="inlineStr">
+        <is>
+          <t>Business phone number for OC's firm.</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="14.25" customHeight="1" s="4">
       <c r="A14" s="9" t="n"/>
       <c r="B14" s="9" t="inlineStr">
         <is>
-          <t>matterdesc</t>
+          <t>plaintifffaxPhone</t>
         </is>
       </c>
       <c r="C14" s="10" t="inlineStr"/>
@@ -771,7 +788,7 @@
       </c>
       <c r="E14" s="9" t="inlineStr">
         <is>
-          <t>Basic description of case/legal service</t>
+          <t>Plaintiff's OC's firm's fax number.</t>
         </is>
       </c>
     </row>
@@ -779,7 +796,7 @@
       <c r="A15" s="9" t="n"/>
       <c r="B15" s="9" t="inlineStr">
         <is>
-          <t>matterid</t>
+          <t>plaintifffaxphone</t>
         </is>
       </c>
       <c r="C15" s="10" t="inlineStr"/>
@@ -790,26 +807,34 @@
       </c>
       <c r="E15" s="9" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>Fax phone number for OC's firm.</t>
         </is>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1" s="4">
-      <c r="A16" s="9" t="inlineStr">
-        <is>
-          <t>Settlement</t>
-        </is>
-      </c>
-      <c r="B16" s="9" t="n"/>
-      <c r="C16" s="12" t="n"/>
-      <c r="D16" s="9" t="n"/>
-      <c r="E16" s="9" t="n"/>
+      <c r="A16" s="9" t="n"/>
+      <c r="B16" s="9" t="inlineStr">
+        <is>
+          <t>plaintifffirmCity</t>
+        </is>
+      </c>
+      <c r="C16" s="12" t="inlineStr"/>
+      <c r="D16" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E16" s="9" t="inlineStr">
+        <is>
+          <t>Plaintiff's OC's firm's city.</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" s="4">
       <c r="A17" s="9" t="n"/>
       <c r="B17" s="9" t="inlineStr">
         <is>
-          <t>testvariable1</t>
+          <t>plaintifffirmSt</t>
         </is>
       </c>
       <c r="C17" s="10" t="inlineStr"/>
@@ -820,89 +845,225 @@
       </c>
       <c r="E17" s="9" t="inlineStr">
         <is>
-          <t>testtest</t>
+          <t>Plaintiff's OC's firm's state situs, all caps: NE or IA</t>
         </is>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1" s="4">
       <c r="A18" s="9" t="n"/>
-      <c r="B18" s="9" t="n"/>
-      <c r="C18" s="10" t="n"/>
-      <c r="D18" s="9" t="n"/>
-      <c r="E18" s="9" t="n"/>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>plaintifffirmZip</t>
+        </is>
+      </c>
+      <c r="C18" s="10" t="inlineStr"/>
+      <c r="D18" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E18" s="9" t="inlineStr">
+        <is>
+          <t>Plaintiff's OC's firm's zip code.</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="14.25" customHeight="1" s="4">
       <c r="A19" s="9" t="n"/>
-      <c r="B19" s="9" t="n"/>
-      <c r="C19" s="10" t="n"/>
-      <c r="D19" s="9" t="n"/>
-      <c r="E19" s="9" t="n"/>
+      <c r="B19" s="9" t="inlineStr">
+        <is>
+          <t>plaintifffirmaddress</t>
+        </is>
+      </c>
+      <c r="C19" s="10" t="inlineStr"/>
+      <c r="D19" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E19" s="9" t="inlineStr">
+        <is>
+          <t>Plaintiff's OC's firm's street address, e.g. "101 Street St., Suite 101"</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="14.25" customHeight="1" s="4">
       <c r="A20" s="9" t="n"/>
-      <c r="B20" s="9" t="n"/>
-      <c r="C20" s="10" t="n"/>
-      <c r="D20" s="9" t="n"/>
-      <c r="E20" s="9" t="n"/>
+      <c r="B20" s="9" t="inlineStr">
+        <is>
+          <t>plaintifffirmcity</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="inlineStr"/>
+      <c r="D20" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E20" s="9" t="inlineStr">
+        <is>
+          <t>City in which opposing party's attorney's firm is.</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="14.25" customHeight="1" s="4">
       <c r="A21" s="9" t="n"/>
-      <c r="B21" s="9" t="n"/>
-      <c r="C21" s="10" t="n"/>
-      <c r="D21" s="9" t="n"/>
-      <c r="E21" s="9" t="n"/>
+      <c r="B21" s="9" t="inlineStr">
+        <is>
+          <t>plaintifffirmname</t>
+        </is>
+      </c>
+      <c r="C21" s="10" t="inlineStr"/>
+      <c r="D21" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E21" s="9" t="inlineStr">
+        <is>
+          <t>Plaintiff's OC's firm's address's zip code.</t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="14.25" customHeight="1" s="4">
       <c r="A22" s="9" t="n"/>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="10" t="n"/>
-      <c r="D22" s="9" t="n"/>
-      <c r="E22" s="9" t="n"/>
+      <c r="B22" s="9" t="inlineStr">
+        <is>
+          <t>plaintifffirmst</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="inlineStr"/>
+      <c r="D22" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E22" s="9" t="inlineStr">
+        <is>
+          <t>State in which OC's firm is in, e.g. NE or IA or WY</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="14.25" customHeight="1" s="4">
       <c r="A23" s="9" t="n"/>
-      <c r="B23" s="9" t="n"/>
-      <c r="C23" s="10" t="n"/>
-      <c r="D23" s="9" t="n"/>
-      <c r="E23" s="9" t="n"/>
+      <c r="B23" s="9" t="inlineStr">
+        <is>
+          <t>plaintiffname</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="inlineStr"/>
+      <c r="D23" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E23" s="9" t="inlineStr">
+        <is>
+          <t>Plaintiff's name as contained in the caption</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="14.25" customHeight="1" s="4">
       <c r="A24" s="9" t="n"/>
-      <c r="B24" s="9" t="n"/>
-      <c r="C24" s="10" t="n"/>
-      <c r="D24" s="9" t="n"/>
-      <c r="E24" s="9" t="n"/>
+      <c r="B24" s="9" t="inlineStr">
+        <is>
+          <t>plaintiffplural</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr"/>
+      <c r="D24" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E24" s="9" t="inlineStr">
+        <is>
+          <t>Whether "Plaintiff" or "Plaintiffs"</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="14.25" customHeight="1" s="4">
       <c r="A25" s="9" t="n"/>
-      <c r="B25" s="9" t="n"/>
-      <c r="C25" s="10" t="n"/>
-      <c r="D25" s="9" t="n"/>
-      <c r="E25" s="9" t="n"/>
+      <c r="B25" s="9" t="inlineStr">
+        <is>
+          <t>plaintiffpossessive</t>
+        </is>
+      </c>
+      <c r="C25" s="10" t="inlineStr"/>
+      <c r="D25" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E25" s="9" t="inlineStr">
+        <is>
+          <t>Type Plaintiff's or Plaintiffs' for possesive.</t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="14.25" customHeight="1" s="4">
       <c r="A26" s="9" t="n"/>
-      <c r="B26" s="9" t="n"/>
-      <c r="C26" s="10" t="n"/>
-      <c r="D26" s="9" t="n"/>
-      <c r="E26" s="9" t="n"/>
+      <c r="B26" s="9" t="inlineStr">
+        <is>
+          <t>plurals</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr"/>
+      <c r="D26" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E26" s="9" t="inlineStr">
+        <is>
+          <t>Pluralizes words following defendant, e.g. Defendant jumps or Defendants jump; type s or leave blank.</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="14.25" customHeight="1" s="4">
       <c r="A27" s="9" t="n"/>
-      <c r="B27" s="9" t="n"/>
-      <c r="C27" s="10" t="n"/>
-      <c r="D27" s="9" t="n"/>
-      <c r="E27" s="9" t="n"/>
+      <c r="B27" s="9" t="inlineStr">
+        <is>
+          <t>servmethod</t>
+        </is>
+      </c>
+      <c r="C27" s="10" t="inlineStr"/>
+      <c r="D27" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E27" s="9" t="inlineStr">
+        <is>
+          <t>Things like e-mail, personal service, e-service.</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="14.25" customHeight="1" s="4">
       <c r="A28" s="9" t="n"/>
-      <c r="B28" s="9" t="n"/>
-      <c r="C28" s="10" t="n"/>
-      <c r="D28" s="9" t="n"/>
-      <c r="E28" s="9" t="n"/>
+      <c r="B28" s="9" t="inlineStr">
+        <is>
+          <t>venue</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="inlineStr"/>
+      <c r="D28" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E28" s="9" t="inlineStr">
+        <is>
+          <t>the county name, e.g. "Garfield County"</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="14.25" customHeight="1" s="4">
-      <c r="A29" s="9" t="n"/>
+      <c r="A29" s="9" t="inlineStr">
+        <is>
+          <t>Client</t>
+        </is>
+      </c>
       <c r="B29" s="9" t="n"/>
       <c r="C29" s="10" t="n"/>
       <c r="D29" s="9" t="n"/>
@@ -910,41 +1071,105 @@
     </row>
     <row r="30" ht="14.25" customHeight="1" s="4">
       <c r="A30" s="9" t="n"/>
-      <c r="B30" s="9" t="n"/>
-      <c r="C30" s="10" t="n"/>
-      <c r="D30" s="9" t="n"/>
-      <c r="E30" s="9" t="n"/>
+      <c r="B30" s="9" t="inlineStr">
+        <is>
+          <t>birthdate</t>
+        </is>
+      </c>
+      <c r="C30" s="10" t="inlineStr"/>
+      <c r="D30" s="9" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="E30" s="9" t="inlineStr">
+        <is>
+          <t>Client's birthday</t>
+        </is>
+      </c>
     </row>
     <row r="31" ht="14.25" customHeight="1" s="4">
       <c r="A31" s="9" t="n"/>
-      <c r="B31" s="9" t="n"/>
-      <c r="C31" s="10" t="n"/>
-      <c r="D31" s="9" t="n"/>
-      <c r="E31" s="9" t="n"/>
+      <c r="B31" s="9" t="inlineStr">
+        <is>
+          <t>firstname</t>
+        </is>
+      </c>
+      <c r="C31" s="10" t="inlineStr"/>
+      <c r="D31" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E31" s="9" t="inlineStr">
+        <is>
+          <t>Client's first name (legal)</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="14.25" customHeight="1" s="4">
       <c r="A32" s="9" t="n"/>
-      <c r="B32" s="9" t="n"/>
-      <c r="C32" s="10" t="n"/>
-      <c r="D32" s="9" t="n"/>
-      <c r="E32" s="9" t="n"/>
+      <c r="B32" s="9" t="inlineStr">
+        <is>
+          <t>lastname</t>
+        </is>
+      </c>
+      <c r="C32" s="10" t="inlineStr"/>
+      <c r="D32" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E32" s="9" t="inlineStr">
+        <is>
+          <t>Client's last name (legal)</t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" s="4">
       <c r="A33" s="9" t="n"/>
-      <c r="B33" s="9" t="n"/>
-      <c r="C33" s="10" t="n"/>
-      <c r="D33" s="9" t="n"/>
-      <c r="E33" s="9" t="n"/>
+      <c r="B33" s="9" t="inlineStr">
+        <is>
+          <t>spousefirstname</t>
+        </is>
+      </c>
+      <c r="C33" s="10" t="inlineStr"/>
+      <c r="D33" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E33" s="9" t="inlineStr">
+        <is>
+          <t>Lauren</t>
+        </is>
+      </c>
     </row>
     <row r="34" ht="14.25" customHeight="1" s="4">
       <c r="A34" s="9" t="n"/>
-      <c r="B34" s="9" t="n"/>
-      <c r="C34" s="10" t="n"/>
-      <c r="D34" s="9" t="n"/>
-      <c r="E34" s="9" t="n"/>
+      <c r="B34" s="9" t="inlineStr">
+        <is>
+          <t>spouselastname</t>
+        </is>
+      </c>
+      <c r="C34" s="10" t="inlineStr"/>
+      <c r="D34" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E34" s="9" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="14.25" customHeight="1" s="4">
-      <c r="A35" s="9" t="n"/>
+      <c r="A35" s="9" t="inlineStr">
+        <is>
+          <t>Derived</t>
+        </is>
+      </c>
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="10" t="n"/>
       <c r="D35" s="9" t="n"/>
@@ -952,27 +1177,67 @@
     </row>
     <row r="36" ht="14.25" customHeight="1" s="4">
       <c r="A36" s="9" t="n"/>
-      <c r="B36" s="9" t="n"/>
-      <c r="C36" s="10" t="n"/>
-      <c r="D36" s="9" t="n"/>
-      <c r="E36" s="9" t="n"/>
+      <c r="B36" s="9" t="inlineStr">
+        <is>
+          <t>defendantcaption</t>
+        </is>
+      </c>
+      <c r="C36" s="10" t="inlineStr"/>
+      <c r="D36" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E36" s="9" t="inlineStr">
+        <is>
+          <t>Derived: wholename_client and wholename_clientspouse</t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="14.25" customHeight="1" s="4">
       <c r="A37" s="9" t="n"/>
-      <c r="B37" s="9" t="n"/>
-      <c r="C37" s="10" t="n"/>
-      <c r="D37" s="9" t="n"/>
-      <c r="E37" s="9" t="n"/>
+      <c r="B37" s="9" t="inlineStr">
+        <is>
+          <t>wholename_client</t>
+        </is>
+      </c>
+      <c r="C37" s="10" t="inlineStr"/>
+      <c r="D37" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E37" s="9" t="inlineStr">
+        <is>
+          <t>Derived: firstname  lastname</t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="14.25" customHeight="1" s="4">
       <c r="A38" s="9" t="n"/>
-      <c r="B38" s="9" t="n"/>
-      <c r="C38" s="10" t="n"/>
-      <c r="D38" s="9" t="n"/>
-      <c r="E38" s="9" t="n"/>
+      <c r="B38" s="9" t="inlineStr">
+        <is>
+          <t>wholename_clientspouse</t>
+        </is>
+      </c>
+      <c r="C38" s="10" t="inlineStr"/>
+      <c r="D38" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E38" s="9" t="inlineStr">
+        <is>
+          <t>Derived: spousefirstname  spouselastname</t>
+        </is>
+      </c>
     </row>
     <row r="39" ht="14.25" customHeight="1" s="4">
-      <c r="A39" s="9" t="n"/>
+      <c r="A39" s="9" t="inlineStr">
+        <is>
+          <t>Internal</t>
+        </is>
+      </c>
       <c r="B39" s="9" t="n"/>
       <c r="C39" s="10" t="n"/>
       <c r="D39" s="9" t="n"/>
@@ -980,17 +1245,41 @@
     </row>
     <row r="40" ht="14.25" customHeight="1" s="4">
       <c r="A40" s="9" t="n"/>
-      <c r="B40" s="9" t="n"/>
-      <c r="C40" s="10" t="n"/>
-      <c r="D40" s="9" t="n"/>
-      <c r="E40" s="9" t="n"/>
+      <c r="B40" s="9" t="inlineStr">
+        <is>
+          <t>matterdesc</t>
+        </is>
+      </c>
+      <c r="C40" s="10" t="inlineStr"/>
+      <c r="D40" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E40" s="9" t="inlineStr">
+        <is>
+          <t>Basic description of case/legal service</t>
+        </is>
+      </c>
     </row>
     <row r="41" ht="14.25" customHeight="1" s="4">
       <c r="A41" s="9" t="n"/>
-      <c r="B41" s="9" t="n"/>
-      <c r="C41" s="10" t="n"/>
-      <c r="D41" s="9" t="n"/>
-      <c r="E41" s="9" t="n"/>
+      <c r="B41" s="9" t="inlineStr">
+        <is>
+          <t>matterid</t>
+        </is>
+      </c>
+      <c r="C41" s="10" t="inlineStr"/>
+      <c r="D41" s="9" t="inlineStr">
+        <is>
+          <t>string</t>
+        </is>
+      </c>
+      <c r="E41" s="9" t="inlineStr">
+        <is>
+          <t>Account/Clio No.</t>
+        </is>
+      </c>
     </row>
     <row r="42" ht="14.25" customHeight="1" s="4">
       <c r="A42" s="9" t="n"/>

</xml_diff>